<commit_message>
Proyecto gestion de incidencias: Modifico la cabecera del excel
</commit_message>
<xml_diff>
--- a/proyectos/gestorDeActuaciones/src/pruebasExcel/prueba1.xlsx
+++ b/proyectos/gestorDeActuaciones/src/pruebasExcel/prueba1.xlsx
@@ -19,90 +19,40 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="D2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
-    Estas incidencias son el id de los casos que enlaza con el código de cliente</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">Cod Incidencia</t>
+  </si>
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
-    <t xml:space="preserve">Teléfono Contacto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo Servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código Incidencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Población Instalación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direccion Instalación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pepito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mijas pueblo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calle de mijas pueblo, 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juanito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuengirola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calle de fuengirola, 67, 1ºA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andres segovia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los boliches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urbanizacion Los boliches, portal 4, 6ºD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fito cabrales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vigo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calle fito y fitipaldis, 45</t>
+    <t xml:space="preserve">Descripción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[333758]Maria Gómez Jimenez-25038550Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alta nuevo numero telefonia fija interna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[333728]Fabiola Cruz Rodriguez – 32038184N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portabilidad numero telefonia fija interna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[333759]Angus Young-25038551Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[333729]Mick Jagger – 32038185N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[333759]Paco de Lucía-25038551Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[333728]Bon Scott – 32038186N</t>
   </si>
 </sst>
 </file>
@@ -135,7 +85,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,12 +96,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4E95D9"/>
         <bgColor rgb="FF3366FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -189,16 +133,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,7 +196,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFC000"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -279,17 +219,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="13.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,94 +240,71 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>285628</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>285663</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>111111111</v>
-      </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>285629</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>266001</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C4" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>285664</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>285630</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C6" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>285665</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>222222222</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>266002</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>333333333</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>266003</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>444444444</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>266004</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>18</v>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -400,6 +315,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>